<commit_message>
Ajout dans les factures producteurs par produits du Quantity string
</commit_message>
<xml_diff>
--- a/src/Stolons/wwwroot/bills/Consumer/1/2016_29_1.xlsx
+++ b/src/Stolons/wwwroot/bills/Consumer/1/2016_29_1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Association Stolons</t>
   </si>
@@ -50,7 +50,7 @@
     <t>Edité le :</t>
   </si>
   <si>
-    <t>20/07/2016 21:29:16</t>
+    <t>22/07/2016 22:10:41</t>
   </si>
   <si>
     <t>Produits de votre panier de la semaine</t>
@@ -83,9 +83,21 @@
     <t>1 pièce</t>
   </si>
   <si>
+    <t>Tomates grappe</t>
+  </si>
+  <si>
+    <t>Au poids par 500 g</t>
+  </si>
+  <si>
+    <t>1,5 Kg</t>
+  </si>
+  <si>
     <t>Salade</t>
   </si>
   <si>
+    <t>2 pièces</t>
+  </si>
+  <si>
     <t>Pomme de terre</t>
   </si>
   <si>
@@ -93,6 +105,12 @@
   </si>
   <si>
     <t>1 Kg</t>
+  </si>
+  <si>
+    <t>Radis</t>
+  </si>
+  <si>
+    <t>Thyn sauvage 2</t>
   </si>
   <si>
     <t xml:space="preserve">TOTAL : </t>
@@ -237,7 +255,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0" view="pageLayout"/>
   </sheetViews>
@@ -406,52 +424,112 @@
         <v>23</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C17" s="4">
-        <v>0.800000011920929</v>
+        <v>1.5</v>
       </c>
       <c r="D17" s="0">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F17" s="13">
         <f>C17*D17</f>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="7">
+      <c r="A18" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="4">
+        <v>0.800000011920929</v>
+      </c>
+      <c r="D18" s="0">
+        <v>2</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="13">
+        <f>C18*D18</f>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="4">
         <v>1.9900000095367432</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D19" s="0">
         <v>1</v>
       </c>
-      <c r="E18" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F18" s="14">
-        <f>C18*D18</f>
-      </c>
-    </row>
-    <row r="19">
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="13">
+        <f>C19*D19</f>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="4">
+        <v>4</v>
+      </c>
+      <c r="D20" s="0">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="13">
+        <f>C20*D20</f>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="7">
+        <v>3</v>
+      </c>
+      <c r="D21" s="6">
+        <v>2</v>
+      </c>
+      <c r="E21" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F19" s="15">
-        <f>SUBTOTAL(9,F16:F18)</f>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="2" t="s">
-        <v>28</v>
+      <c r="F21" s="14">
+        <f>C21*D21</f>
+      </c>
+    </row>
+    <row r="22">
+      <c r="E22" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" s="15">
+        <f>SUBTOTAL(9,F16:F21)</f>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>